<commit_message>
cambios de base de datos
</commit_message>
<xml_diff>
--- a/Tickers.xlsx
+++ b/Tickers.xlsx
@@ -537,8 +537,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="dd.mm"/>
-    <numFmt numFmtId="165" formatCode="d.m"/>
+    <numFmt numFmtId="164" formatCode="d.m"/>
+    <numFmt numFmtId="165" formatCode="dd.mm"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -818,8 +818,8 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
-        <v>43557.0</v>
+      <c r="B3" s="2">
+        <v>2.04</v>
       </c>
     </row>
     <row r="4">
@@ -1106,7 +1106,7 @@
       <c r="A39" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <v>43800.0</v>
       </c>
     </row>
@@ -1114,7 +1114,7 @@
       <c r="A40" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="3">
         <v>43770.0</v>
       </c>
     </row>
@@ -1122,7 +1122,7 @@
       <c r="A41" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>43770.0</v>
       </c>
     </row>
@@ -1130,7 +1130,7 @@
       <c r="A42" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="4">
         <v>43709.0</v>
       </c>
     </row>
@@ -1138,7 +1138,7 @@
       <c r="A43" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="4">
         <v>43678.0</v>
       </c>
     </row>
@@ -1146,7 +1146,7 @@
       <c r="A44" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="4">
         <v>43647.0</v>
       </c>
     </row>
@@ -1154,7 +1154,7 @@
       <c r="A45" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="4">
         <v>43647.0</v>
       </c>
     </row>
@@ -1162,7 +1162,7 @@
       <c r="A46" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="4">
         <v>43647.0</v>
       </c>
     </row>
@@ -1170,7 +1170,7 @@
       <c r="A47" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="4">
         <v>43617.0</v>
       </c>
     </row>
@@ -1178,7 +1178,7 @@
       <c r="A48" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="4">
         <v>43617.0</v>
       </c>
     </row>
@@ -1186,7 +1186,7 @@
       <c r="A49" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="4">
         <v>43617.0</v>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       <c r="A50" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="4">
         <v>43586.0</v>
       </c>
     </row>
@@ -1202,7 +1202,7 @@
       <c r="A51" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="4">
         <v>43525.0</v>
       </c>
     </row>

</xml_diff>